<commit_message>
Aggiornamento file per test case id 191
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/dedalus/caleido_fse20_connector/2023/accreditamento-checklist_V7.1.1.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/dedalus/caleido_fse20_connector/2023/accreditamento-checklist_V7.1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia.trama\OneDrive - Dedalus S.p.A\Documenti\PROGETTI\FSE\2.0\accreditamento\TEST CALEIDO\Versione 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A740D735-E0E8-459F-AA54-9A593755A7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23E9524-E6E8-44BE-B9D9-FF60CB86EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="972" windowWidth="22596" windowHeight="11148" tabRatio="207" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="444" yWindow="768" windowWidth="22596" windowHeight="11148" tabRatio="207" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="249">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1088,6 +1088,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.4.3.8.52c6ec5df15550425bc47dcab3f83e8a885842df51838ff2a3338f965cd9f91a.0bda25fddc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-28T11:20:05Z</t>
+  </si>
+  <si>
+    <t>249a7475aef0cdac</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.8.5345cd66a1c56d61a2d12bc5fc09e41fcc3845815ad2ddefb38d3924cb97039d.fc82b113e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3041,10 +3050,10 @@
   <dimension ref="A1:T850"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5215,16 +5224,16 @@
         <v>198</v>
       </c>
       <c r="F55" s="17">
-        <v>45012</v>
+        <v>45013</v>
       </c>
       <c r="G55" s="32" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="J55" s="19" t="s">
         <v>47</v>
@@ -21009,15 +21018,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -21248,6 +21248,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -21260,14 +21269,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21286,6 +21287,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>